<commit_message>
refactoring code to reduce the size of XX_sorter.py
</commit_message>
<xml_diff>
--- a/EE_Programs.xlsx
+++ b/EE_Programs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\steve\OneDrive\20110706\TaiGer_Transcript-Program_Comparer\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0CED78A4-AA70-4053-965C-4D8F38FE1955}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68FCF381-23D7-44E6-A889-DDF03CEA503A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="21825" yWindow="-16350" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-6975" yWindow="-16320" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Program_choosing" sheetId="1" r:id="rId1"/>
@@ -372,7 +372,7 @@
   <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>